<commit_message>
Python code completed (Brute force)
</commit_message>
<xml_diff>
--- a/Hesperia.xlsx
+++ b/Hesperia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11360" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="14820" yWindow="0" windowWidth="14000" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Master Scores" sheetId="6" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -553,10 +553,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -845,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="F16">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6">

</xml_diff>

<commit_message>
Added output to Excel file function
</commit_message>
<xml_diff>
--- a/Hesperia.xlsx
+++ b/Hesperia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="0" windowWidth="14000" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Master Scores" sheetId="6" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -553,10 +553,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -925,7 +925,7 @@
         <v>4</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated output - correct package numbers
</commit_message>
<xml_diff>
--- a/Hesperia.xlsx
+++ b/Hesperia.xlsx
@@ -526,7 +526,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -613,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>1</v>

</xml_diff>